<commit_message>
Added Aspen Hand Support
</commit_message>
<xml_diff>
--- a/Documentation/Working_Documents/Aspen_Joystick_BOM.xlsx
+++ b/Documentation/Working_Documents/Aspen_Joystick_BOM.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://neilsquiresoc.sharepoint.com/sites/MMC-RD/Shared Documents/RD 22-05 OpenAT Joysticks/Designs/Active Projects/Sliding Analog Thumbstick/Aspen_Sliding_Joystick_v1.0/Aspen_Sliding_Joystick/Documentation/Working_Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://neilsquiresoc-my.sharepoint.com/personal/josiev_neilsquire_ca/Documents/Documents/GitHub/Aspen-Sliding-Joystick/Documentation/Working_Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="296" documentId="8_{FFCF63BE-D2B6-4D57-AB99-D42729B3DC72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5AB58359-9FC4-47BE-89C8-B9DAB89C8BD3}"/>
+  <xr:revisionPtr revIDLastSave="304" documentId="8_{FFCF63BE-D2B6-4D57-AB99-D42729B3DC72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66B4B3F5-1A98-427E-A681-AFBFB7C7D2B8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">BOM!$A$1:$L$42</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">BOM!$A$1:$L$43</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">BOM!$1:$2</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="76">
   <si>
     <t>Unit Cost</t>
   </si>
@@ -279,6 +279,9 @@
   </si>
   <si>
     <t>https://www.digikey.ca/en/products/detail/tensility-international-corp/10-00341/2350244</t>
+  </si>
+  <si>
+    <t>(Optional) Aspen_Hand_Support</t>
   </si>
 </sst>
 </file>
@@ -866,10 +869,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N42"/>
+  <dimension ref="A1:N43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -915,20 +918,20 @@
         <v>67</v>
       </c>
       <c r="I2" s="20">
-        <f>SUM(I5:I13,J15:J25)</f>
+        <f>SUM(I5:I13,J15:J26)</f>
         <v>20.0275</v>
       </c>
       <c r="J2" s="4">
-        <f>SUM(J5:J13,J15:J25)</f>
+        <f>SUM(J5:J13,J15:J26)</f>
         <v>20.0275</v>
       </c>
       <c r="K2" s="14">
-        <f>SUM(H15:H25)/60</f>
+        <f>SUM(H15:H26)/60</f>
         <v>1.55</v>
       </c>
       <c r="L2" s="5">
-        <f>SUM(E15:E20)</f>
-        <v>29.500000000000004</v>
+        <f>SUM(E15:E21)</f>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1323,15 +1326,15 @@
         <v>28</v>
       </c>
       <c r="H16">
-        <f t="shared" ref="H16:H24" si="4">F16*D16</f>
+        <f t="shared" ref="H16:H25" si="4">F16*D16</f>
         <v>28</v>
       </c>
       <c r="I16" s="12">
-        <f t="shared" ref="I16:I25" si="5">(E16/1000)*$C$13</f>
+        <f t="shared" ref="I16:I26" si="5">(E16/1000)*$C$13</f>
         <v>0.11499999999999999</v>
       </c>
       <c r="J16" s="18">
-        <f t="shared" ref="J16:J25" si="6">I16*D16</f>
+        <f t="shared" ref="J16:J26" si="6">I16*D16</f>
         <v>0.11499999999999999</v>
       </c>
     </row>
@@ -1424,7 +1427,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="C20" t="s">
         <v>25</v>
@@ -1433,10 +1436,10 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>0.6</v>
+        <v>38.5</v>
       </c>
       <c r="F20">
-        <v>8</v>
+        <v>189</v>
       </c>
       <c r="H20">
         <f t="shared" si="4"/>
@@ -1444,7 +1447,7 @@
       </c>
       <c r="I20" s="12">
         <f t="shared" si="5"/>
-        <v>1.4999999999999999E-2</v>
+        <v>0.96250000000000002</v>
       </c>
       <c r="J20" s="18">
         <f t="shared" si="6"/>
@@ -1453,7 +1456,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C21" t="s">
         <v>25</v>
@@ -1462,10 +1465,10 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>1.7</v>
+        <v>0.6</v>
       </c>
       <c r="F21">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="H21">
         <f t="shared" si="4"/>
@@ -1473,7 +1476,7 @@
       </c>
       <c r="I21" s="12">
         <f t="shared" si="5"/>
-        <v>4.2499999999999996E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="J21" s="18">
         <f t="shared" si="6"/>
@@ -1482,7 +1485,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C22" t="s">
         <v>25</v>
@@ -1491,10 +1494,10 @@
         <v>0</v>
       </c>
       <c r="E22">
-        <v>4.9000000000000004</v>
+        <v>1.7</v>
       </c>
       <c r="F22">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="H22">
         <f t="shared" si="4"/>
@@ -1502,7 +1505,7 @@
       </c>
       <c r="I22" s="12">
         <f t="shared" si="5"/>
-        <v>0.12250000000000001</v>
+        <v>4.2499999999999996E-2</v>
       </c>
       <c r="J22" s="18">
         <f t="shared" si="6"/>
@@ -1511,7 +1514,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C23" t="s">
         <v>25</v>
@@ -1520,10 +1523,10 @@
         <v>0</v>
       </c>
       <c r="E23">
-        <v>1.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="F23">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="H23">
         <f t="shared" si="4"/>
@@ -1531,7 +1534,7 @@
       </c>
       <c r="I23" s="12">
         <f t="shared" si="5"/>
-        <v>3.7499999999999999E-2</v>
+        <v>0.12250000000000001</v>
       </c>
       <c r="J23" s="18">
         <f t="shared" si="6"/>
@@ -1540,7 +1543,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C24" t="s">
         <v>25</v>
@@ -1549,10 +1552,10 @@
         <v>0</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="F24">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H24">
         <f t="shared" si="4"/>
@@ -1560,7 +1563,7 @@
       </c>
       <c r="I24" s="12">
         <f t="shared" si="5"/>
-        <v>2.5000000000000001E-2</v>
+        <v>3.7499999999999999E-2</v>
       </c>
       <c r="J24" s="18">
         <f t="shared" si="6"/>
@@ -1568,163 +1571,156 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B25" s="10"/>
+      <c r="B25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>10</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="I25" s="12">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="J25" s="18">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B26" s="10"/>
+      <c r="I26" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J26" s="18">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="35" t="s">
+      <c r="B27" s="10"/>
+    </row>
+    <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="9"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>31</v>
-      </c>
+      <c r="B28" s="36"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
         <v>58</v>
       </c>
-      <c r="K33" s="7" t="s">
+      <c r="K34" s="7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="31" t="s">
+    <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="32"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
-      <c r="J35" s="9"/>
-      <c r="K35" s="9"/>
-      <c r="L35" s="9"/>
-      <c r="M35" s="9"/>
-      <c r="N35" s="9"/>
-    </row>
-    <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="16" t="s">
+      <c r="B36" s="32"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="9"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="9"/>
+      <c r="N36" s="9"/>
+    </row>
+    <row r="37" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="22" t="s">
+      <c r="B37" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C37" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D37" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="E37" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F36" s="6" t="s">
+      <c r="F37" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G36" s="6" t="s">
+      <c r="G37" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H36" s="6" t="s">
+      <c r="H37" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I36" s="6" t="s">
+      <c r="I37" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="J36" s="6" t="s">
+      <c r="J37" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="K36" s="16" t="s">
+      <c r="K37" s="16" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>38</v>
-      </c>
-      <c r="C37" t="s">
-        <v>18</v>
-      </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37">
-        <v>1</v>
-      </c>
-      <c r="F37" s="8">
-        <v>1.5</v>
-      </c>
-      <c r="G37" s="17">
-        <f t="shared" ref="G37:G38" si="7">IF(E37&gt;0,ROUNDUP(D37/E37,0),0)</f>
-        <v>1</v>
-      </c>
-      <c r="H37" s="19">
-        <f t="shared" ref="H37:H41" si="8">IF(E37&gt;0,F37/E37,0)</f>
-        <v>1.5</v>
-      </c>
-      <c r="I37" s="19">
-        <f t="shared" ref="I37:I41" si="9">H37*D37</f>
-        <v>1.5</v>
-      </c>
-      <c r="J37" s="18">
-        <f t="shared" ref="J37:J41" si="10">G37*F37</f>
-        <v>1.5</v>
-      </c>
-      <c r="K37" s="7" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C38" t="s">
         <v>18</v>
@@ -1736,68 +1732,71 @@
         <v>1</v>
       </c>
       <c r="F38" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="G38" s="17">
+        <f t="shared" ref="G38:G39" si="7">IF(E38&gt;0,ROUNDUP(D38/E38,0),0)</f>
+        <v>1</v>
+      </c>
+      <c r="H38" s="19">
+        <f t="shared" ref="H38:H42" si="8">IF(E38&gt;0,F38/E38,0)</f>
+        <v>1.5</v>
+      </c>
+      <c r="I38" s="19">
+        <f t="shared" ref="I38:I42" si="9">H38*D38</f>
+        <v>1.5</v>
+      </c>
+      <c r="J38" s="18">
+        <f t="shared" ref="J38:J42" si="10">G38*F38</f>
+        <v>1.5</v>
+      </c>
+      <c r="K38" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>29</v>
+      </c>
+      <c r="C39" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39" s="8">
         <v>2.5</v>
       </c>
-      <c r="G38" s="17">
+      <c r="G39" s="17">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="H38" s="19">
+      <c r="H39" s="19">
         <f t="shared" si="8"/>
         <v>2.5</v>
       </c>
-      <c r="I38" s="19">
+      <c r="I39" s="19">
         <f t="shared" si="9"/>
         <v>2.5</v>
       </c>
-      <c r="J38" s="18">
+      <c r="J39" s="18">
         <f t="shared" si="10"/>
         <v>2.5</v>
       </c>
-      <c r="K38" s="7" t="s">
+      <c r="K39" s="7" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>51</v>
-      </c>
-      <c r="C39" t="s">
-        <v>18</v>
-      </c>
-      <c r="D39">
-        <v>0.5</v>
-      </c>
-      <c r="E39">
-        <v>1</v>
-      </c>
-      <c r="F39" s="25">
-        <v>2.89</v>
-      </c>
-      <c r="G39" s="26">
-        <f t="shared" ref="G39:G41" si="11">IF(E39&gt;0,ROUNDUP(D39/E39,0),0)</f>
-        <v>1</v>
-      </c>
-      <c r="H39" s="12">
-        <f t="shared" si="8"/>
-        <v>2.89</v>
-      </c>
-      <c r="I39" s="12">
-        <f t="shared" si="9"/>
-        <v>1.4450000000000001</v>
-      </c>
-      <c r="J39" s="18">
-        <f t="shared" si="10"/>
-        <v>2.89</v>
-      </c>
-      <c r="K39" s="7" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>51</v>
       </c>
+      <c r="C40" t="s">
+        <v>18</v>
+      </c>
       <c r="D40">
         <v>0.5</v>
       </c>
@@ -1805,121 +1804,154 @@
         <v>1</v>
       </c>
       <c r="F40" s="25">
-        <v>6.71</v>
+        <v>2.89</v>
       </c>
       <c r="G40" s="26">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="G40:G42" si="11">IF(E40&gt;0,ROUNDUP(D40/E40,0),0)</f>
         <v>1</v>
       </c>
       <c r="H40" s="12">
         <f t="shared" si="8"/>
-        <v>6.71</v>
+        <v>2.89</v>
       </c>
       <c r="I40" s="12">
         <f t="shared" si="9"/>
-        <v>3.355</v>
+        <v>1.4450000000000001</v>
       </c>
       <c r="J40" s="18">
         <f t="shared" si="10"/>
-        <v>6.71</v>
+        <v>2.89</v>
       </c>
       <c r="K40" s="7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>52</v>
-      </c>
-      <c r="C41" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="D41">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="E41">
-        <v>340</v>
-      </c>
-      <c r="F41" s="24">
-        <v>22.14</v>
-      </c>
-      <c r="G41" s="17">
+        <v>1</v>
+      </c>
+      <c r="F41" s="25">
+        <v>6.71</v>
+      </c>
+      <c r="G41" s="26">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="H41" s="12">
         <f t="shared" si="8"/>
-        <v>6.511764705882353E-2</v>
+        <v>6.71</v>
       </c>
       <c r="I41" s="12">
         <f t="shared" si="9"/>
-        <v>0.26047058823529412</v>
+        <v>3.355</v>
       </c>
       <c r="J41" s="18">
         <f t="shared" si="10"/>
-        <v>22.14</v>
+        <v>6.71</v>
       </c>
       <c r="K41" s="7" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42">
+        <v>4</v>
+      </c>
+      <c r="E42">
+        <v>340</v>
+      </c>
+      <c r="F42" s="24">
+        <v>22.14</v>
+      </c>
+      <c r="G42" s="17">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="H42" s="12">
+        <f t="shared" si="8"/>
+        <v>6.511764705882353E-2</v>
+      </c>
+      <c r="I42" s="12">
+        <f t="shared" si="9"/>
+        <v>0.26047058823529412</v>
+      </c>
+      <c r="J42" s="18">
+        <f t="shared" si="10"/>
+        <v>22.14</v>
+      </c>
+      <c r="K42" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
         <v>72</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>73</v>
       </c>
-      <c r="D42">
-        <v>1</v>
-      </c>
-      <c r="E42">
-        <v>1</v>
-      </c>
-      <c r="F42" s="8">
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43" s="8">
         <v>7.19</v>
       </c>
-      <c r="G42" s="17">
-        <v>1</v>
-      </c>
-      <c r="H42" s="19">
-        <f>IF(E42&gt;0,F42/E42,0)</f>
+      <c r="G43" s="17">
+        <v>1</v>
+      </c>
+      <c r="H43" s="19">
+        <f>IF(E43&gt;0,F43/E43,0)</f>
         <v>7.19</v>
       </c>
-      <c r="I42" s="19">
-        <f>H42*D42</f>
+      <c r="I43" s="19">
+        <f>H43*D43</f>
         <v>7.19</v>
       </c>
-      <c r="J42" s="18">
-        <f>G42*F42</f>
+      <c r="J43" s="18">
+        <f>G43*F43</f>
         <v>7.19</v>
       </c>
-      <c r="K42" s="7" t="s">
+      <c r="K43" s="7" t="s">
         <v>74</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K5" r:id="rId1" xr:uid="{2BDEC5B6-9C5C-4DF3-B048-251F8DB1F9AA}"/>
     <hyperlink ref="K6" r:id="rId2" xr:uid="{D2382A15-9AC3-4E43-BA16-A9ED529FF8B4}"/>
-    <hyperlink ref="K37" r:id="rId3" xr:uid="{96DE242E-188A-4B6A-88C9-4BD647E2C8E7}"/>
-    <hyperlink ref="K38" r:id="rId4" xr:uid="{329487A5-33CB-43A8-87AE-830E4120192A}"/>
-    <hyperlink ref="K39" r:id="rId5" location="sku383491 " xr:uid="{78075580-FCB1-472A-B19F-C78FD2B8257C}"/>
+    <hyperlink ref="K38" r:id="rId3" xr:uid="{96DE242E-188A-4B6A-88C9-4BD647E2C8E7}"/>
+    <hyperlink ref="K39" r:id="rId4" xr:uid="{329487A5-33CB-43A8-87AE-830E4120192A}"/>
+    <hyperlink ref="K40" r:id="rId5" location="sku383491 " xr:uid="{78075580-FCB1-472A-B19F-C78FD2B8257C}"/>
     <hyperlink ref="K10" r:id="rId6" xr:uid="{46A12388-0439-42C4-9F35-824318D34603}"/>
-    <hyperlink ref="K33" r:id="rId7" xr:uid="{B0336E92-9552-45FA-A8B4-4F1203D569EF}"/>
-    <hyperlink ref="K41" r:id="rId8" xr:uid="{6635064D-C9CA-415A-9952-F9C05894ABE2}"/>
+    <hyperlink ref="K34" r:id="rId7" xr:uid="{B0336E92-9552-45FA-A8B4-4F1203D569EF}"/>
+    <hyperlink ref="K42" r:id="rId8" xr:uid="{6635064D-C9CA-415A-9952-F9C05894ABE2}"/>
     <hyperlink ref="K9" r:id="rId9" xr:uid="{6C723921-38D4-4AA8-85E0-326D2023B051}"/>
     <hyperlink ref="K8" r:id="rId10" xr:uid="{D4B5BE68-BB9C-4824-A2EC-5657A09A97E0}"/>
-    <hyperlink ref="K40" r:id="rId11" xr:uid="{2CBFA260-558B-40C8-BDCC-BF92FDDFEEFD}"/>
+    <hyperlink ref="K41" r:id="rId11" xr:uid="{2CBFA260-558B-40C8-BDCC-BF92FDDFEEFD}"/>
     <hyperlink ref="K7" r:id="rId12" xr:uid="{60C4109D-04E2-45A9-A045-507D86216D53}"/>
-    <hyperlink ref="K42" r:id="rId13" xr:uid="{898F5857-1857-45A7-954C-B69870F0884B}"/>
+    <hyperlink ref="K43" r:id="rId13" xr:uid="{898F5857-1857-45A7-954C-B69870F0884B}"/>
   </hyperlinks>
   <printOptions gridLines="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -1928,6 +1960,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="72c39c84-b0a3-45a2-a38c-ff46bb47f11f" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B51EC7ECFAC78D4E8EF6CBAFFF0B3505" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c16a8de1b3ad07fcfe40131daee80152">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e" xmlns:ns3="72c39c84-b0a3-45a2-a38c-ff46bb47f11f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="85720a748046338a72a4f25fe522aa39" ns2:_="" ns3:_="">
     <xsd:import namespace="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e"/>
@@ -2176,27 +2228,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="72c39c84-b0a3-45a2-a38c-ff46bb47f11f" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="72c39c84-b0a3-45a2-a38c-ff46bb47f11f"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4740145F-09D2-466B-B9A2-2798696B0ADF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7F61F1-65EA-4381-A5A1-B24E039B79DF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2213,29 +2270,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="72c39c84-b0a3-45a2-a38c-ff46bb47f11f"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4740145F-09D2-466B-B9A2-2798696B0ADF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>